<commit_message>
FPNCT c-obj mod complete
completed adjustment of select c-objects in series FPNCT and modified oblique synapses for first round of in-silico testing
</commit_message>
<xml_diff>
--- a/XRZCT/190225_XRZCT_dch_oblq_test/192507_XRZCT_dch_oblq_test.xlsx
+++ b/XRZCT/190225_XRZCT_dch_oblq_test/192507_XRZCT_dch_oblq_test.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Harris Lab Repos\CA1_2hr\XRZCT\190225_XRZCT_dch_oblq_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF41D43-A2C4-492A-9267-B41280EB3B99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF6F3EB-96FE-4C41-A76C-07517A1DE20B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45240" yWindow="1680" windowWidth="8880" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XRZCT" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">XRZCT!$A$1:$AE$103</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -78,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="2" shapeId="0" xr:uid="{B7092E80-FE31-4EC0-8DCC-EC9A4752C9E8}">
+    <comment ref="G4" authorId="2" shapeId="0" xr:uid="{B7092E80-FE31-4EC0-8DCC-EC9A4752C9E8}">
       <text>
         <r>
           <rPr>
@@ -103,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T11" authorId="2" shapeId="0" xr:uid="{A2476B1D-B736-48BC-8980-33BBA1072534}">
+    <comment ref="T8" authorId="2" shapeId="0" xr:uid="{A2476B1D-B736-48BC-8980-33BBA1072534}">
       <text>
         <r>
           <rPr>
@@ -128,7 +137,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="T18" authorId="2" shapeId="0" xr:uid="{51E6FB4F-E35A-454A-86D6-B89E4877F8E8}">
+    <comment ref="T11" authorId="2" shapeId="0" xr:uid="{166D037A-099A-4611-A401-BB881026A37C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Dakota H:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Synapse is oblique</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T22" authorId="2" shapeId="0" xr:uid="{51E6FB4F-E35A-454A-86D6-B89E4877F8E8}">
       <text>
         <r>
           <rPr>
@@ -153,31 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T23" authorId="2" shapeId="0" xr:uid="{166D037A-099A-4611-A401-BB881026A37C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Dakota H:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Synapse is oblique</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T24" authorId="2" shapeId="0" xr:uid="{1B593F1A-176A-467C-9A20-02E25162DFAB}">
+    <comment ref="T26" authorId="2" shapeId="0" xr:uid="{1B593F1A-176A-467C-9A20-02E25162DFAB}">
       <text>
         <r>
           <rPr>
@@ -281,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="427">
   <si>
     <t>Experiment</t>
   </si>
@@ -1543,9 +1552,6 @@
     <t>Original Reconstruct cfa value ("ground truth")</t>
   </si>
   <si>
-    <t>Blender cfa value (from c-object)</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -1553,6 +1559,18 @@
   </si>
   <si>
     <t>o -&gt; x</t>
+  </si>
+  <si>
+    <t>Reconstruct cfa value</t>
+  </si>
+  <si>
+    <t>Original Blender c-object intersection area</t>
+  </si>
+  <si>
+    <t>Resectioned Blender c-object intersection area</t>
+  </si>
+  <si>
+    <t>test avg psd width</t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1899,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2165,6 +2183,11 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2531,9 +2554,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AE103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V12" sqref="V12"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W43" sqref="W43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2626,16 +2649,20 @@
         <v>19</v>
       </c>
       <c r="U1" s="111" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="V1" s="111" t="s">
         <v>419</v>
       </c>
       <c r="W1" s="111" t="s">
-        <v>420</v>
-      </c>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="112"/>
+        <v>423</v>
+      </c>
+      <c r="X1" s="111" t="s">
+        <v>424</v>
+      </c>
+      <c r="Y1" s="112" t="s">
+        <v>425</v>
+      </c>
       <c r="Z1" s="112"/>
       <c r="AA1" s="93"/>
     </row>
@@ -2735,10 +2762,13 @@
       <c r="S3" s="63"/>
       <c r="T3" s="94"/>
       <c r="U3" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V3" s="98">
         <v>1</v>
+      </c>
+      <c r="W3" s="98">
+        <v>8.5116600000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
@@ -2752,53 +2782,56 @@
         <v>22</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="F4" s="96" t="s">
-        <v>160</v>
-      </c>
-      <c r="G4" s="108" t="s">
-        <v>423</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="97" t="s">
+        <v>59</v>
       </c>
       <c r="H4" s="97" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="I4" s="97" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="J4" s="66" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="L4" s="12">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="M4" s="12">
-        <v>159</v>
-      </c>
-      <c r="N4" s="13">
-        <v>383</v>
+        <v>138</v>
+      </c>
+      <c r="N4" s="12">
+        <v>103</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="63"/>
+      <c r="S4" s="65"/>
       <c r="T4" s="94"/>
       <c r="U4" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V4" s="98">
         <v>1</v>
+      </c>
+      <c r="W4" s="98">
+        <v>1.3870800000000001E-2</v>
       </c>
       <c r="X4" s="99"/>
       <c r="Y4" s="99"/>
@@ -2816,119 +2849,120 @@
         <v>22</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="E5" s="96" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="F5" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="108" t="s">
-        <v>423</v>
+      <c r="G5" s="97" t="s">
+        <v>59</v>
       </c>
       <c r="H5" s="97" t="s">
-        <v>135</v>
+        <v>191</v>
       </c>
       <c r="I5" s="97" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="J5" s="66" t="s">
-        <v>137</v>
+        <v>200</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="L5" s="12">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="M5" s="12">
-        <v>210</v>
-      </c>
-      <c r="N5" s="12">
-        <v>594</v>
+        <v>158</v>
+      </c>
+      <c r="N5" s="13">
+        <v>309</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="P5" s="11"/>
-      <c r="Q5" s="10" t="s">
-        <v>139</v>
-      </c>
+      <c r="Q5" s="10"/>
       <c r="R5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S5" s="65"/>
-      <c r="T5" s="94" t="s">
-        <v>140</v>
-      </c>
+      <c r="S5" s="63"/>
+      <c r="T5" s="94"/>
       <c r="U5" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V5" s="98">
         <v>1</v>
       </c>
+      <c r="W5" s="98">
+        <v>9.0225700000000006E-2</v>
+      </c>
+      <c r="X5" s="99"/>
     </row>
     <row r="6" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="114" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="95" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" s="96" t="s">
-        <v>182</v>
-      </c>
-      <c r="F6" s="96" t="s">
+      <c r="D6" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="116" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="97" t="s">
-        <v>183</v>
-      </c>
-      <c r="I6" s="97" t="s">
-        <v>184</v>
+      <c r="H6" s="117" t="s">
+        <v>222</v>
+      </c>
+      <c r="I6" s="117" t="s">
+        <v>223</v>
       </c>
       <c r="J6" s="66" t="s">
-        <v>185</v>
+        <v>224</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="L6" s="12">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="M6" s="12">
-        <v>138</v>
-      </c>
-      <c r="N6" s="12">
-        <v>103</v>
+        <v>129</v>
+      </c>
+      <c r="N6" s="13">
+        <v>1049</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>63</v>
       </c>
       <c r="P6" s="11"/>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="12" t="s">
+        <v>226</v>
+      </c>
       <c r="R6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S6" s="65"/>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94" t="s">
-        <v>421</v>
-      </c>
-      <c r="V6" s="98">
-        <v>1</v>
-      </c>
-      <c r="X6" s="99"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="114"/>
+      <c r="U6" s="114"/>
+      <c r="V6" s="118">
+        <v>0</v>
+      </c>
+      <c r="W6" s="118"/>
+      <c r="X6" s="118"/>
       <c r="Y6" s="99"/>
       <c r="Z6" s="99"/>
       <c r="AA6" s="99"/>
@@ -2944,118 +2978,125 @@
         <v>22</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="E7" s="96" t="s">
-        <v>199</v>
+        <v>58</v>
       </c>
       <c r="F7" s="96" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G7" s="97" t="s">
         <v>59</v>
       </c>
       <c r="H7" s="97" t="s">
-        <v>191</v>
+        <v>60</v>
       </c>
       <c r="I7" s="97" t="s">
-        <v>192</v>
+        <v>53</v>
       </c>
       <c r="J7" s="66" t="s">
-        <v>200</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>201</v>
+        <v>61</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>62</v>
       </c>
       <c r="L7" s="12">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="M7" s="12">
-        <v>158</v>
-      </c>
-      <c r="N7" s="13">
-        <v>309</v>
+        <v>183</v>
+      </c>
+      <c r="N7" s="12">
+        <v>604</v>
       </c>
       <c r="O7" s="12" t="s">
         <v>63</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="10"/>
-      <c r="R7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="S7" s="63"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="65"/>
       <c r="T7" s="94"/>
       <c r="U7" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V7" s="98">
         <v>1</v>
+      </c>
+      <c r="W7" s="98">
+        <v>0.25147199999999997</v>
       </c>
       <c r="X7" s="99"/>
       <c r="Y7" s="99"/>
       <c r="Z7" s="99"/>
       <c r="AA7" s="99"/>
     </row>
-    <row r="8" spans="1:27" s="118" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="114" t="s">
+    <row r="8" spans="1:27" s="125" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="94" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="115" t="s">
-        <v>220</v>
-      </c>
-      <c r="E8" s="116" t="s">
-        <v>221</v>
-      </c>
-      <c r="F8" s="116" t="s">
+      <c r="D8" s="95" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="117" t="s">
-        <v>222</v>
-      </c>
-      <c r="I8" s="117" t="s">
-        <v>223</v>
+      <c r="H8" s="97" t="s">
+        <v>244</v>
+      </c>
+      <c r="I8" s="97" t="s">
+        <v>245</v>
       </c>
       <c r="J8" s="66" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="L8" s="12">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="M8" s="12">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="N8" s="13">
-        <v>1049</v>
+        <v>806</v>
       </c>
       <c r="O8" s="12" t="s">
         <v>63</v>
       </c>
       <c r="P8" s="11"/>
-      <c r="Q8" s="12" t="s">
-        <v>226</v>
-      </c>
+      <c r="Q8" s="10"/>
       <c r="R8" s="10" t="s">
         <v>28</v>
       </c>
       <c r="S8" s="63"/>
-      <c r="T8" s="114"/>
-      <c r="U8" s="114"/>
-      <c r="V8" s="118">
-        <v>0</v>
-      </c>
+      <c r="T8" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="U8" s="94" t="s">
+        <v>420</v>
+      </c>
+      <c r="V8" s="98">
+        <v>1</v>
+      </c>
+      <c r="W8" s="98">
+        <v>5.05011E-2</v>
+      </c>
+      <c r="X8" s="99"/>
     </row>
     <row r="9" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94" t="s">
@@ -3068,53 +3109,56 @@
         <v>22</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>234</v>
+        <v>279</v>
       </c>
       <c r="E9" s="96" t="s">
-        <v>235</v>
+        <v>280</v>
       </c>
       <c r="F9" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="108" t="s">
-        <v>423</v>
+      <c r="G9" s="97" t="s">
+        <v>59</v>
       </c>
       <c r="H9" s="97" t="s">
-        <v>236</v>
+        <v>281</v>
       </c>
       <c r="I9" s="97" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="J9" s="66" t="s">
-        <v>238</v>
+        <v>283</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>239</v>
+        <v>284</v>
       </c>
       <c r="L9" s="12">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="M9" s="12">
-        <v>134</v>
-      </c>
-      <c r="N9" s="12">
-        <v>252</v>
+        <v>118</v>
+      </c>
+      <c r="N9" s="13">
+        <v>631</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S9" s="65"/>
+      <c r="S9" s="63"/>
       <c r="T9" s="94"/>
       <c r="U9" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V9" s="98">
         <v>1</v>
+      </c>
+      <c r="W9" s="98">
+        <v>0.13083</v>
       </c>
     </row>
     <row r="10" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
@@ -3128,51 +3172,58 @@
         <v>22</v>
       </c>
       <c r="D10" s="95" t="s">
-        <v>57</v>
+        <v>312</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>58</v>
+        <v>313</v>
       </c>
       <c r="F10" s="96" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="G10" s="97" t="s">
         <v>59</v>
       </c>
       <c r="H10" s="97" t="s">
-        <v>60</v>
+        <v>314</v>
       </c>
       <c r="I10" s="97" t="s">
-        <v>53</v>
+        <v>315</v>
       </c>
       <c r="J10" s="66" t="s">
-        <v>61</v>
+        <v>316</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>62</v>
+        <v>317</v>
       </c>
       <c r="L10" s="12">
+        <v>111</v>
+      </c>
+      <c r="M10" s="12">
+        <v>143</v>
+      </c>
+      <c r="N10" s="13">
         <v>119</v>
       </c>
-      <c r="M10" s="12">
-        <v>183</v>
-      </c>
-      <c r="N10" s="12">
-        <v>604</v>
-      </c>
       <c r="O10" s="12" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="P10" s="11"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="94"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="63"/>
+      <c r="T10" s="94" t="s">
+        <v>318</v>
+      </c>
       <c r="U10" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V10" s="98">
         <v>1</v>
+      </c>
+      <c r="W10" s="98">
+        <v>0.108665</v>
       </c>
       <c r="X10" s="99"/>
       <c r="Y10" s="99"/>
@@ -3180,47 +3231,47 @@
       <c r="AA10" s="99"/>
     </row>
     <row r="11" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="119" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="95" t="s">
-        <v>242</v>
-      </c>
-      <c r="E11" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="F11" s="96" t="s">
+      <c r="D11" s="120" t="s">
+        <v>346</v>
+      </c>
+      <c r="E11" s="121" t="s">
+        <v>347</v>
+      </c>
+      <c r="F11" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="97" t="s">
+      <c r="G11" s="122" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="97" t="s">
-        <v>244</v>
-      </c>
-      <c r="I11" s="97" t="s">
-        <v>245</v>
+      <c r="H11" s="122" t="s">
+        <v>348</v>
+      </c>
+      <c r="I11" s="122" t="s">
+        <v>349</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>247</v>
+        <v>350</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>351</v>
       </c>
       <c r="L11" s="12">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="M11" s="12">
-        <v>99</v>
-      </c>
-      <c r="N11" s="13">
-        <v>806</v>
+        <v>149</v>
+      </c>
+      <c r="N11" s="12">
+        <v>479</v>
       </c>
       <c r="O11" s="12" t="s">
         <v>63</v>
@@ -3230,17 +3281,20 @@
       <c r="R11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S11" s="63"/>
-      <c r="T11" s="94" t="s">
-        <v>248</v>
-      </c>
-      <c r="U11" s="94" t="s">
-        <v>421</v>
-      </c>
-      <c r="V11" s="98">
-        <v>1</v>
-      </c>
-      <c r="X11" s="99"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="119" t="s">
+        <v>352</v>
+      </c>
+      <c r="U11" s="119" t="s">
+        <v>420</v>
+      </c>
+      <c r="V11" s="123">
+        <v>0</v>
+      </c>
+      <c r="W11" s="123">
+        <v>8.6648600000000006E-2</v>
+      </c>
+      <c r="X11" s="124"/>
       <c r="Y11" s="99"/>
       <c r="Z11" s="99"/>
       <c r="AA11" s="99"/>
@@ -3256,37 +3310,37 @@
         <v>22</v>
       </c>
       <c r="D12" s="95" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="F12" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="108" t="s">
-        <v>423</v>
+      <c r="G12" s="97" t="s">
+        <v>59</v>
       </c>
       <c r="H12" s="97" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="I12" s="97" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="L12" s="12">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="M12" s="12">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="N12" s="13">
-        <v>658</v>
+        <v>321</v>
       </c>
       <c r="O12" s="12" t="s">
         <v>27</v>
@@ -3297,16 +3351,16 @@
         <v>28</v>
       </c>
       <c r="S12" s="63"/>
-      <c r="T12" s="94" t="s">
-        <v>268</v>
-      </c>
+      <c r="T12" s="94"/>
       <c r="U12" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V12" s="98">
         <v>1</v>
       </c>
-      <c r="X12" s="99"/>
+      <c r="W12" s="98">
+        <v>0.10194</v>
+      </c>
       <c r="Y12" s="99"/>
       <c r="Z12" s="99"/>
       <c r="AA12" s="99"/>
@@ -3322,10 +3376,10 @@
         <v>22</v>
       </c>
       <c r="D13" s="95" t="s">
-        <v>279</v>
+        <v>98</v>
       </c>
       <c r="E13" s="96" t="s">
-        <v>280</v>
+        <v>99</v>
       </c>
       <c r="F13" s="96" t="s">
         <v>23</v>
@@ -3334,25 +3388,25 @@
         <v>59</v>
       </c>
       <c r="H13" s="97" t="s">
-        <v>281</v>
+        <v>100</v>
       </c>
       <c r="I13" s="97" t="s">
-        <v>282</v>
+        <v>95</v>
       </c>
       <c r="J13" s="66" t="s">
-        <v>283</v>
+        <v>101</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>284</v>
+        <v>102</v>
       </c>
       <c r="L13" s="12">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="M13" s="12">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="N13" s="13">
-        <v>631</v>
+        <v>133</v>
       </c>
       <c r="O13" s="12" t="s">
         <v>27</v>
@@ -3365,10 +3419,13 @@
       <c r="S13" s="63"/>
       <c r="T13" s="94"/>
       <c r="U13" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V13" s="98">
         <v>1</v>
+      </c>
+      <c r="W13" s="98">
+        <v>0.132878</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
@@ -3382,37 +3439,37 @@
         <v>22</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>285</v>
+        <v>158</v>
       </c>
       <c r="E14" s="96" t="s">
-        <v>286</v>
+        <v>159</v>
       </c>
       <c r="F14" s="96" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="G14" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H14" s="97" t="s">
-        <v>287</v>
+        <v>161</v>
       </c>
       <c r="I14" s="97" t="s">
-        <v>288</v>
+        <v>162</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>289</v>
+        <v>163</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>290</v>
+        <v>164</v>
       </c>
       <c r="L14" s="12">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="M14" s="12">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="N14" s="13">
-        <v>798</v>
+        <v>383</v>
       </c>
       <c r="O14" s="12" t="s">
         <v>27</v>
@@ -3425,7 +3482,7 @@
       <c r="S14" s="63"/>
       <c r="T14" s="94"/>
       <c r="U14" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V14" s="98">
         <v>1</v>
@@ -3446,55 +3503,58 @@
         <v>22</v>
       </c>
       <c r="D15" s="95" t="s">
-        <v>291</v>
+        <v>134</v>
       </c>
       <c r="E15" s="96" t="s">
-        <v>292</v>
+        <v>137</v>
       </c>
       <c r="F15" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H15" s="97" t="s">
-        <v>293</v>
+        <v>135</v>
       </c>
       <c r="I15" s="97" t="s">
-        <v>294</v>
+        <v>136</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>295</v>
+        <v>137</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>296</v>
+        <v>138</v>
       </c>
       <c r="L15" s="12">
-        <v>117</v>
+        <v>1</v>
       </c>
       <c r="M15" s="12">
-        <v>143</v>
-      </c>
-      <c r="N15" s="13">
-        <v>496</v>
+        <v>210</v>
+      </c>
+      <c r="N15" s="12">
+        <v>594</v>
       </c>
       <c r="O15" s="12" t="s">
         <v>27</v>
       </c>
       <c r="P15" s="11"/>
-      <c r="Q15" s="10"/>
+      <c r="Q15" s="10" t="s">
+        <v>139</v>
+      </c>
       <c r="R15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S15" s="63"/>
-      <c r="T15" s="94"/>
+      <c r="S15" s="65"/>
+      <c r="T15" s="94" t="s">
+        <v>140</v>
+      </c>
       <c r="U15" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V15" s="98">
         <v>1</v>
       </c>
-      <c r="X15" s="99"/>
       <c r="Y15" s="99"/>
       <c r="Z15" s="99"/>
       <c r="AA15" s="99"/>
@@ -3510,57 +3570,54 @@
         <v>22</v>
       </c>
       <c r="D16" s="95" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="E16" s="96" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="F16" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H16" s="97" t="s">
-        <v>191</v>
+        <v>236</v>
       </c>
       <c r="I16" s="97" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
       <c r="J16" s="66" t="s">
-        <v>193</v>
+        <v>238</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
       <c r="L16" s="12">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="M16" s="12">
-        <v>158</v>
-      </c>
-      <c r="N16" s="13">
-        <v>37</v>
+        <v>134</v>
+      </c>
+      <c r="N16" s="12">
+        <v>252</v>
       </c>
       <c r="O16" s="12" t="s">
         <v>63</v>
       </c>
       <c r="P16" s="11"/>
-      <c r="Q16" s="10" t="s">
-        <v>195</v>
-      </c>
+      <c r="Q16" s="10"/>
       <c r="R16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S16" s="63"/>
+      <c r="S16" s="65"/>
       <c r="T16" s="94"/>
       <c r="U16" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V16" s="98">
         <v>1</v>
       </c>
-      <c r="X16" s="99"/>
       <c r="Y16" s="99"/>
       <c r="Z16" s="99"/>
       <c r="AA16" s="99"/>
@@ -3618,54 +3675,52 @@
         <v>22</v>
       </c>
       <c r="D18" s="95" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="E18" s="96" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="F18" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H18" s="97" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="I18" s="97" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="L18" s="12">
-        <v>145</v>
+        <v>106</v>
       </c>
       <c r="M18" s="12">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="N18" s="13">
-        <v>342</v>
+        <v>658</v>
       </c>
       <c r="O18" s="12" t="s">
         <v>27</v>
       </c>
       <c r="P18" s="11"/>
-      <c r="Q18" s="10" t="s">
-        <v>303</v>
-      </c>
+      <c r="Q18" s="10"/>
       <c r="R18" s="10" t="s">
         <v>28</v>
       </c>
       <c r="S18" s="63"/>
       <c r="T18" s="94" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="U18" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V18" s="98">
         <v>1</v>
@@ -3686,52 +3741,50 @@
         <v>22</v>
       </c>
       <c r="D19" s="95" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="E19" s="96" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="F19" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="97" t="s">
-        <v>59</v>
+      <c r="G19" s="108" t="s">
+        <v>422</v>
       </c>
       <c r="H19" s="97" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
       <c r="I19" s="97" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="J19" s="66" t="s">
-        <v>316</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>317</v>
+        <v>289</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>290</v>
       </c>
       <c r="L19" s="12">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M19" s="12">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="N19" s="13">
-        <v>119</v>
+        <v>798</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>27</v>
       </c>
       <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
+      <c r="Q19" s="10"/>
       <c r="R19" s="10" t="s">
         <v>28</v>
       </c>
       <c r="S19" s="63"/>
-      <c r="T19" s="94" t="s">
-        <v>318</v>
-      </c>
+      <c r="T19" s="94"/>
       <c r="U19" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V19" s="98">
         <v>1</v>
@@ -3752,37 +3805,37 @@
         <v>22</v>
       </c>
       <c r="D20" s="95" t="s">
-        <v>321</v>
+        <v>291</v>
       </c>
       <c r="E20" s="96" t="s">
-        <v>322</v>
+        <v>292</v>
       </c>
       <c r="F20" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H20" s="97" t="s">
-        <v>323</v>
+        <v>293</v>
       </c>
       <c r="I20" s="97" t="s">
-        <v>324</v>
+        <v>294</v>
       </c>
       <c r="J20" s="66" t="s">
-        <v>325</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>326</v>
+        <v>295</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>296</v>
       </c>
       <c r="L20" s="12">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="M20" s="12">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="N20" s="13">
-        <v>232</v>
+        <v>496</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>27</v>
@@ -3795,7 +3848,7 @@
       <c r="S20" s="63"/>
       <c r="T20" s="94"/>
       <c r="U20" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V20" s="98">
         <v>1</v>
@@ -3816,50 +3869,52 @@
         <v>22</v>
       </c>
       <c r="D21" s="95" t="s">
-        <v>330</v>
+        <v>189</v>
       </c>
       <c r="E21" s="96" t="s">
-        <v>331</v>
+        <v>190</v>
       </c>
       <c r="F21" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H21" s="97" t="s">
-        <v>332</v>
+        <v>191</v>
       </c>
       <c r="I21" s="97" t="s">
-        <v>333</v>
+        <v>192</v>
       </c>
       <c r="J21" s="66" t="s">
-        <v>334</v>
+        <v>193</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>335</v>
+        <v>194</v>
       </c>
       <c r="L21" s="12">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="M21" s="12">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="N21" s="13">
-        <v>269</v>
+        <v>37</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>63</v>
       </c>
       <c r="P21" s="11"/>
-      <c r="Q21" s="10"/>
+      <c r="Q21" s="10" t="s">
+        <v>195</v>
+      </c>
       <c r="R21" s="10" t="s">
         <v>28</v>
       </c>
       <c r="S21" s="63"/>
       <c r="T21" s="94"/>
       <c r="U21" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V21" s="98">
         <v>1</v>
@@ -3880,50 +3935,54 @@
         <v>22</v>
       </c>
       <c r="D22" s="95" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="E22" s="96" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
       <c r="F22" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H22" s="97" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
       <c r="I22" s="97" t="s">
+        <v>300</v>
+      </c>
+      <c r="J22" s="66" t="s">
+        <v>301</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="L22" s="12">
+        <v>145</v>
+      </c>
+      <c r="M22" s="12">
+        <v>174</v>
+      </c>
+      <c r="N22" s="13">
         <v>342</v>
       </c>
-      <c r="J22" s="66" t="s">
-        <v>343</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="L22" s="12">
-        <v>113</v>
-      </c>
-      <c r="M22" s="12">
-        <v>147</v>
-      </c>
-      <c r="N22" s="12">
-        <v>200</v>
-      </c>
       <c r="O22" s="12" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="P22" s="11"/>
-      <c r="Q22" s="10"/>
+      <c r="Q22" s="10" t="s">
+        <v>303</v>
+      </c>
       <c r="R22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S22" s="65"/>
-      <c r="T22" s="94"/>
+      <c r="S22" s="63"/>
+      <c r="T22" s="94" t="s">
+        <v>304</v>
+      </c>
       <c r="U22" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V22" s="98">
         <v>1</v>
@@ -3933,71 +3992,70 @@
       <c r="Z22" s="99"/>
       <c r="AA22" s="99"/>
     </row>
-    <row r="23" spans="1:27" s="123" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="119" t="s">
+    <row r="23" spans="1:27" s="127" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="119" t="s">
+      <c r="B23" s="94" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="120" t="s">
-        <v>346</v>
-      </c>
-      <c r="E23" s="121" t="s">
-        <v>347</v>
-      </c>
-      <c r="F23" s="121" t="s">
+      <c r="D23" s="95" t="s">
+        <v>321</v>
+      </c>
+      <c r="E23" s="96" t="s">
+        <v>322</v>
+      </c>
+      <c r="F23" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="122" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="122" t="s">
-        <v>348</v>
-      </c>
-      <c r="I23" s="122" t="s">
-        <v>349</v>
+      <c r="G23" s="108" t="s">
+        <v>422</v>
+      </c>
+      <c r="H23" s="97" t="s">
+        <v>323</v>
+      </c>
+      <c r="I23" s="97" t="s">
+        <v>324</v>
       </c>
       <c r="J23" s="66" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="L23" s="12">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="M23" s="12">
-        <v>149</v>
-      </c>
-      <c r="N23" s="12">
-        <v>479</v>
+        <v>126</v>
+      </c>
+      <c r="N23" s="13">
+        <v>232</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S23" s="65"/>
-      <c r="T23" s="119" t="s">
-        <v>352</v>
-      </c>
-      <c r="U23" s="119" t="s">
-        <v>421</v>
-      </c>
-      <c r="V23" s="123">
-        <v>0</v>
-      </c>
-      <c r="X23" s="124"/>
-      <c r="Y23" s="124"/>
-      <c r="Z23" s="124"/>
-      <c r="AA23" s="124"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="94"/>
+      <c r="U23" s="94" t="s">
+        <v>420</v>
+      </c>
+      <c r="V23" s="98">
+        <v>1</v>
+      </c>
+      <c r="W23" s="98"/>
+      <c r="X23" s="99"/>
+      <c r="Y23" s="126"/>
+      <c r="Z23" s="126"/>
+      <c r="AA23" s="126"/>
     </row>
     <row r="24" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94" t="s">
@@ -4010,52 +4068,50 @@
         <v>22</v>
       </c>
       <c r="D24" s="95" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="E24" s="96" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="F24" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H24" s="97" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="I24" s="97" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="J24" s="66" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="L24" s="12">
+        <v>65</v>
+      </c>
+      <c r="M24" s="12">
         <v>142</v>
       </c>
-      <c r="M24" s="12">
-        <v>160</v>
-      </c>
-      <c r="N24" s="12">
-        <v>511</v>
+      <c r="N24" s="13">
+        <v>269</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S24" s="65"/>
-      <c r="T24" s="94" t="s">
-        <v>362</v>
-      </c>
+      <c r="S24" s="63"/>
+      <c r="T24" s="94"/>
       <c r="U24" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V24" s="98">
         <v>1</v>
@@ -4076,40 +4132,40 @@
         <v>22</v>
       </c>
       <c r="D25" s="95" t="s">
-        <v>176</v>
+        <v>339</v>
       </c>
       <c r="E25" s="96" t="s">
-        <v>177</v>
+        <v>340</v>
       </c>
       <c r="F25" s="96" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H25" s="97" t="s">
-        <v>178</v>
+        <v>341</v>
       </c>
       <c r="I25" s="97" t="s">
-        <v>173</v>
+        <v>342</v>
       </c>
       <c r="J25" s="66" t="s">
-        <v>179</v>
+        <v>343</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>180</v>
+        <v>344</v>
       </c>
       <c r="L25" s="12">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="M25" s="12">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N25" s="12">
-        <v>363</v>
+        <v>200</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="P25" s="11"/>
       <c r="Q25" s="10"/>
@@ -4119,11 +4175,12 @@
       <c r="S25" s="65"/>
       <c r="T25" s="94"/>
       <c r="U25" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V25" s="98">
         <v>1</v>
       </c>
+      <c r="X25" s="99"/>
     </row>
     <row r="26" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="94" t="s">
@@ -4136,37 +4193,37 @@
         <v>22</v>
       </c>
       <c r="D26" s="95" t="s">
-        <v>272</v>
+        <v>356</v>
       </c>
       <c r="E26" s="96" t="s">
-        <v>273</v>
+        <v>357</v>
       </c>
       <c r="F26" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="97" t="s">
-        <v>59</v>
+      <c r="G26" s="108" t="s">
+        <v>422</v>
       </c>
       <c r="H26" s="97" t="s">
-        <v>274</v>
+        <v>358</v>
       </c>
       <c r="I26" s="97" t="s">
-        <v>269</v>
+        <v>359</v>
       </c>
       <c r="J26" s="66" t="s">
-        <v>275</v>
+        <v>360</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>276</v>
+        <v>361</v>
       </c>
       <c r="L26" s="12">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="M26" s="12">
-        <v>111</v>
-      </c>
-      <c r="N26" s="13">
-        <v>321</v>
+        <v>160</v>
+      </c>
+      <c r="N26" s="12">
+        <v>511</v>
       </c>
       <c r="O26" s="12" t="s">
         <v>27</v>
@@ -4176,14 +4233,17 @@
       <c r="R26" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S26" s="63"/>
-      <c r="T26" s="94"/>
+      <c r="S26" s="65"/>
+      <c r="T26" s="94" t="s">
+        <v>362</v>
+      </c>
       <c r="U26" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V26" s="98">
         <v>1</v>
       </c>
+      <c r="X26" s="99"/>
     </row>
     <row r="27" spans="1:27" s="98" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="94" t="s">
@@ -4196,37 +4256,37 @@
         <v>22</v>
       </c>
       <c r="D27" s="95" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="E27" s="96" t="s">
-        <v>99</v>
+        <v>177</v>
       </c>
       <c r="F27" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="97" t="s">
-        <v>59</v>
+      <c r="G27" s="108" t="s">
+        <v>422</v>
       </c>
       <c r="H27" s="97" t="s">
-        <v>100</v>
+        <v>178</v>
       </c>
       <c r="I27" s="97" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
       <c r="J27" s="66" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="L27" s="12">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="M27" s="12">
-        <v>104</v>
-      </c>
-      <c r="N27" s="13">
-        <v>133</v>
+        <v>145</v>
+      </c>
+      <c r="N27" s="12">
+        <v>363</v>
       </c>
       <c r="O27" s="12" t="s">
         <v>27</v>
@@ -4236,10 +4296,10 @@
       <c r="R27" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S27" s="63"/>
+      <c r="S27" s="65"/>
       <c r="T27" s="94"/>
       <c r="U27" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V27" s="98">
         <v>1</v>
@@ -4265,7 +4325,7 @@
         <v>23</v>
       </c>
       <c r="G28" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H28" s="97" t="s">
         <v>386</v>
@@ -4301,7 +4361,7 @@
         <v>390</v>
       </c>
       <c r="U28" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V28" s="98">
         <v>1</v>
@@ -4416,7 +4476,7 @@
         <v>23</v>
       </c>
       <c r="G31" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H31" s="97" t="s">
         <v>398</v>
@@ -4450,7 +4510,7 @@
         <v>402</v>
       </c>
       <c r="U31" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V31" s="98">
         <v>1</v>
@@ -4480,7 +4540,7 @@
         <v>23</v>
       </c>
       <c r="G32" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H32" s="97" t="s">
         <v>405</v>
@@ -4512,7 +4572,7 @@
       <c r="S32" s="63"/>
       <c r="T32" s="94"/>
       <c r="U32" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V32" s="98">
         <v>1</v>
@@ -4542,7 +4602,7 @@
         <v>23</v>
       </c>
       <c r="G33" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H33" s="97" t="s">
         <v>411</v>
@@ -4574,7 +4634,7 @@
       <c r="S33" s="63"/>
       <c r="T33" s="94"/>
       <c r="U33" s="94" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V33" s="98">
         <v>1</v>
@@ -7564,8 +7624,8 @@
       <sortCondition ref="G2:G103"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:W101">
-    <sortCondition ref="D1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:X101">
+    <sortCondition ref="G1"/>
   </sortState>
   <conditionalFormatting sqref="U1:U1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="y">
@@ -7576,4 +7636,80 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A73CF7B-357C-44F3-AED7-87CDAFAD304A}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2.9100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2.86E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.86E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.4299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2.4400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.3800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.1989999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3.2460000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3.2939999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>AVERAGE(A2:A11)</f>
+        <v>2.8268999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>